<commit_message>
Jessie added new data
</commit_message>
<xml_diff>
--- a/data/rrv_ipm_trial_2021.xlsx
+++ b/data/rrv_ipm_trial_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/afife_ufl_edu/Documents/DISSERTATION/MANUSCRIPT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="867" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A05C005E-9FDD-4172-8EE8-7351C512B6FE}"/>
+  <xr:revisionPtr revIDLastSave="868" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EA59112-9BC3-464F-A945-2180E2F7B774}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -489,20 +489,22 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -521,7 +523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>485</v>
       </c>
@@ -541,7 +543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>486</v>
       </c>
@@ -561,7 +563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>487</v>
       </c>
@@ -581,7 +583,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>488</v>
       </c>
@@ -601,7 +603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>489</v>
       </c>
@@ -621,7 +623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>490</v>
       </c>
@@ -641,7 +643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>491</v>
       </c>
@@ -661,7 +663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>492</v>
       </c>
@@ -681,7 +683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>493</v>
       </c>
@@ -701,7 +703,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>494</v>
       </c>
@@ -721,7 +723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>495</v>
       </c>
@@ -741,7 +743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>496</v>
       </c>
@@ -761,7 +763,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>497</v>
       </c>
@@ -781,7 +783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>498</v>
       </c>
@@ -801,7 +803,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>499</v>
       </c>
@@ -821,7 +823,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>500</v>
       </c>
@@ -841,7 +843,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>501</v>
       </c>
@@ -861,7 +863,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>502</v>
       </c>
@@ -881,7 +883,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>503</v>
       </c>
@@ -901,7 +903,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>504</v>
       </c>
@@ -921,7 +923,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>505</v>
       </c>
@@ -941,7 +943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>506</v>
       </c>
@@ -961,7 +963,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>507</v>
       </c>
@@ -981,7 +983,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>508</v>
       </c>
@@ -1001,7 +1003,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>509</v>
       </c>
@@ -1021,7 +1023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>510</v>
       </c>
@@ -1041,7 +1043,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>511</v>
       </c>
@@ -1061,7 +1063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>512</v>
       </c>
@@ -1081,7 +1083,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>513</v>
       </c>
@@ -1101,7 +1103,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>514</v>
       </c>
@@ -1121,7 +1123,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>515</v>
       </c>
@@ -1141,7 +1143,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>516</v>
       </c>
@@ -1161,7 +1163,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>517</v>
       </c>
@@ -1181,7 +1183,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>518</v>
       </c>
@@ -1201,7 +1203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>519</v>
       </c>
@@ -1221,7 +1223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>520</v>
       </c>
@@ -1241,7 +1243,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>521</v>
       </c>
@@ -1261,7 +1263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>522</v>
       </c>
@@ -1281,7 +1283,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>523</v>
       </c>
@@ -1301,7 +1303,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>524</v>
       </c>
@@ -1321,7 +1323,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>525</v>
       </c>
@@ -1341,7 +1343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>526</v>
       </c>
@@ -1361,7 +1363,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>527</v>
       </c>
@@ -1381,7 +1383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>528</v>
       </c>
@@ -1401,7 +1403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>529</v>
       </c>
@@ -1421,7 +1423,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>530</v>
       </c>
@@ -1441,7 +1443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>531</v>
       </c>
@@ -1461,7 +1463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>532</v>
       </c>
@@ -1481,7 +1483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>533</v>
       </c>
@@ -1501,7 +1503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>534</v>
       </c>
@@ -1521,7 +1523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>535</v>
       </c>
@@ -1541,7 +1543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>536</v>
       </c>
@@ -1561,7 +1563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>537</v>
       </c>
@@ -1581,7 +1583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>538</v>
       </c>
@@ -1601,7 +1603,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>539</v>
       </c>
@@ -1621,7 +1623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>540</v>
       </c>
@@ -1641,7 +1643,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>541</v>
       </c>
@@ -1661,7 +1663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>542</v>
       </c>
@@ -1681,7 +1683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>543</v>
       </c>
@@ -1701,7 +1703,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>544</v>
       </c>
@@ -1721,7 +1723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>545</v>
       </c>
@@ -1741,7 +1743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>546</v>
       </c>
@@ -1761,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>547</v>
       </c>
@@ -1781,7 +1783,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>548</v>
       </c>
@@ -1801,7 +1803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>549</v>
       </c>
@@ -1821,7 +1823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>550</v>
       </c>
@@ -1841,7 +1843,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>551</v>
       </c>
@@ -1861,7 +1863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>552</v>
       </c>
@@ -1881,7 +1883,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>553</v>
       </c>
@@ -1901,7 +1903,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>554</v>
       </c>
@@ -1921,7 +1923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>555</v>
       </c>
@@ -1941,7 +1943,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>556</v>
       </c>
@@ -1961,7 +1963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>557</v>
       </c>
@@ -1981,7 +1983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>558</v>
       </c>
@@ -2001,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>559</v>
       </c>
@@ -2021,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>560</v>
       </c>
@@ -2041,7 +2043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>561</v>
       </c>
@@ -2061,7 +2063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>562</v>
       </c>
@@ -2081,7 +2083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>563</v>
       </c>
@@ -2101,7 +2103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>564</v>
       </c>
@@ -2121,7 +2123,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>565</v>
       </c>
@@ -2141,7 +2143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>566</v>
       </c>
@@ -2161,7 +2163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>567</v>
       </c>
@@ -2181,7 +2183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>568</v>
       </c>
@@ -2201,7 +2203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>569</v>
       </c>
@@ -2221,7 +2223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>570</v>
       </c>
@@ -2241,7 +2243,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>571</v>
       </c>
@@ -2261,7 +2263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>572</v>
       </c>
@@ -2281,7 +2283,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>573</v>
       </c>
@@ -2301,7 +2303,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>574</v>
       </c>
@@ -2321,7 +2323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>575</v>
       </c>
@@ -2341,7 +2343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>576</v>
       </c>
@@ -2361,7 +2363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>577</v>
       </c>
@@ -2381,7 +2383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>578</v>
       </c>
@@ -2401,7 +2403,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>579</v>
       </c>
@@ -2421,7 +2423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>580</v>
       </c>
@@ -2441,7 +2443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>581</v>
       </c>
@@ -2461,7 +2463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>582</v>
       </c>
@@ -2481,7 +2483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>583</v>
       </c>
@@ -2501,7 +2503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>584</v>
       </c>
@@ -2521,7 +2523,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>585</v>
       </c>
@@ -2541,7 +2543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>586</v>
       </c>
@@ -2561,7 +2563,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>587</v>
       </c>
@@ -2581,7 +2583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>588</v>
       </c>
@@ -2601,7 +2603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>589</v>
       </c>
@@ -2621,7 +2623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>590</v>
       </c>
@@ -2641,7 +2643,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>591</v>
       </c>
@@ -2661,7 +2663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>592</v>
       </c>
@@ -2681,7 +2683,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>593</v>
       </c>
@@ -2701,7 +2703,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>594</v>
       </c>
@@ -2721,7 +2723,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>595</v>
       </c>
@@ -2741,7 +2743,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>596</v>
       </c>
@@ -2761,7 +2763,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>597</v>
       </c>
@@ -2781,7 +2783,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>598</v>
       </c>
@@ -2801,7 +2803,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>599</v>
       </c>
@@ -2821,7 +2823,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>600</v>
       </c>
@@ -2841,7 +2843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>601</v>
       </c>
@@ -2861,7 +2863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>602</v>
       </c>
@@ -2881,7 +2883,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>603</v>
       </c>
@@ -2901,7 +2903,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>604</v>
       </c>
@@ -2921,7 +2923,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>605</v>
       </c>
@@ -2941,7 +2943,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>606</v>
       </c>
@@ -2961,7 +2963,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>607</v>
       </c>
@@ -2981,7 +2983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>608</v>
       </c>
@@ -3001,7 +3003,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>609</v>
       </c>
@@ -3021,7 +3023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>610</v>
       </c>
@@ -3041,7 +3043,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>611</v>
       </c>
@@ -3061,7 +3063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>612</v>
       </c>
@@ -3081,7 +3083,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>613</v>
       </c>
@@ -3101,7 +3103,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>614</v>
       </c>
@@ -3121,7 +3123,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>615</v>
       </c>
@@ -3141,7 +3143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>616</v>
       </c>
@@ -3161,7 +3163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>617</v>
       </c>
@@ -3181,7 +3183,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>618</v>
       </c>
@@ -3201,7 +3203,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>619</v>
       </c>
@@ -3221,7 +3223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>620</v>
       </c>
@@ -3241,7 +3243,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>621</v>
       </c>
@@ -3261,7 +3263,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>622</v>
       </c>
@@ -3281,7 +3283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>623</v>
       </c>
@@ -3301,7 +3303,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>624</v>
       </c>
@@ -3321,7 +3323,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>625</v>
       </c>
@@ -3341,7 +3343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>626</v>
       </c>
@@ -3361,7 +3363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>627</v>
       </c>
@@ -3381,7 +3383,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>628</v>
       </c>
@@ -3401,7 +3403,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>629</v>
       </c>
@@ -3421,7 +3423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>630</v>
       </c>
@@ -3441,7 +3443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>631</v>
       </c>
@@ -3461,7 +3463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>632</v>
       </c>
@@ -3481,7 +3483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>633</v>
       </c>
@@ -3501,7 +3503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>634</v>
       </c>
@@ -3521,7 +3523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>635</v>
       </c>
@@ -3541,7 +3543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>636</v>
       </c>
@@ -3561,7 +3563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>637</v>
       </c>
@@ -3581,7 +3583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>638</v>
       </c>
@@ -3601,7 +3603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>639</v>
       </c>
@@ -3621,7 +3623,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>640</v>
       </c>
@@ -3641,7 +3643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>641</v>
       </c>
@@ -3661,7 +3663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>642</v>
       </c>
@@ -3681,7 +3683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>643</v>
       </c>
@@ -3701,7 +3703,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>644</v>
       </c>
@@ -3721,7 +3723,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>645</v>
       </c>
@@ -3741,7 +3743,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>646</v>
       </c>
@@ -3761,7 +3763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>647</v>
       </c>
@@ -3781,7 +3783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>648</v>
       </c>
@@ -3801,7 +3803,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>649</v>
       </c>
@@ -3821,7 +3823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>650</v>
       </c>
@@ -3841,7 +3843,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>651</v>
       </c>
@@ -3861,7 +3863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>652</v>
       </c>
@@ -3881,7 +3883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>653</v>
       </c>
@@ -3901,7 +3903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>654</v>
       </c>
@@ -3921,7 +3923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>655</v>
       </c>
@@ -3941,7 +3943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>656</v>
       </c>
@@ -3961,7 +3963,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>657</v>
       </c>
@@ -3981,7 +3983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>658</v>
       </c>
@@ -4001,7 +4003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>659</v>
       </c>
@@ -4021,7 +4023,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>660</v>
       </c>
@@ -4041,7 +4043,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>661</v>
       </c>
@@ -4061,7 +4063,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>662</v>
       </c>
@@ -4081,7 +4083,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>663</v>
       </c>
@@ -4101,7 +4103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>664</v>
       </c>
@@ -4121,7 +4123,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>665</v>
       </c>
@@ -4141,7 +4143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>666</v>
       </c>
@@ -4161,7 +4163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>667</v>
       </c>
@@ -4181,7 +4183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>668</v>
       </c>
@@ -4194,8 +4196,14 @@
       <c r="D185">
         <v>6.1950000000000003</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E185">
+        <v>63</v>
+      </c>
+      <c r="F185">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>669</v>
       </c>
@@ -4208,8 +4216,14 @@
       <c r="D186">
         <v>5.47</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E186">
+        <v>50</v>
+      </c>
+      <c r="F186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>670</v>
       </c>
@@ -4222,8 +4236,14 @@
       <c r="D187">
         <v>4.3630000000000004</v>
       </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E187">
+        <v>40</v>
+      </c>
+      <c r="F187">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>671</v>
       </c>
@@ -4236,8 +4256,14 @@
       <c r="D188">
         <v>7.1680000000000001</v>
       </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E188">
+        <v>0</v>
+      </c>
+      <c r="F188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>672</v>
       </c>
@@ -4250,8 +4276,14 @@
       <c r="D189">
         <v>3.86</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E189">
+        <v>47</v>
+      </c>
+      <c r="F189">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>673</v>
       </c>
@@ -4264,8 +4296,14 @@
       <c r="D190">
         <v>7.5960000000000001</v>
       </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E190">
+        <v>25</v>
+      </c>
+      <c r="F190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>674</v>
       </c>
@@ -4278,8 +4316,14 @@
       <c r="D191">
         <v>6.5350000000000001</v>
       </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E191">
+        <v>43</v>
+      </c>
+      <c r="F191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>675</v>
       </c>
@@ -4292,8 +4336,14 @@
       <c r="D192">
         <v>3.72</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E192">
+        <v>0</v>
+      </c>
+      <c r="F192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>676</v>
       </c>
@@ -4306,8 +4356,14 @@
       <c r="D193">
         <v>5.6909999999999998</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E193">
+        <v>15</v>
+      </c>
+      <c r="F193">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>677</v>
       </c>
@@ -4320,8 +4376,14 @@
       <c r="D194">
         <v>6.7160000000000002</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E194">
+        <v>0</v>
+      </c>
+      <c r="F194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>678</v>
       </c>
@@ -4334,8 +4396,14 @@
       <c r="D195">
         <v>12.686999999999999</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E195">
+        <v>44</v>
+      </c>
+      <c r="F195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>679</v>
       </c>
@@ -4348,8 +4416,14 @@
       <c r="D196">
         <v>15.287000000000001</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E196">
+        <v>19</v>
+      </c>
+      <c r="F196">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>680</v>
       </c>
@@ -4362,8 +4436,14 @@
       <c r="D197">
         <v>17.001999999999999</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E197">
+        <v>69</v>
+      </c>
+      <c r="F197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>681</v>
       </c>
@@ -4376,8 +4456,14 @@
       <c r="D198">
         <v>13.518000000000001</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E198">
+        <v>40</v>
+      </c>
+      <c r="F198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>682</v>
       </c>
@@ -4390,8 +4476,14 @@
       <c r="D199">
         <v>6.2750000000000004</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E199">
+        <v>132</v>
+      </c>
+      <c r="F199">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>683</v>
       </c>
@@ -4404,8 +4496,14 @@
       <c r="D200">
         <v>6.3780000000000001</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E200">
+        <v>2</v>
+      </c>
+      <c r="F200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>684</v>
       </c>
@@ -4418,8 +4516,14 @@
       <c r="D201">
         <v>9.625</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E201">
+        <v>117</v>
+      </c>
+      <c r="F201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>685</v>
       </c>
@@ -4432,8 +4536,14 @@
       <c r="D202">
         <v>15.278</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E202">
+        <v>97</v>
+      </c>
+      <c r="F202">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>686</v>
       </c>
@@ -4446,8 +4556,14 @@
       <c r="D203">
         <v>11.034000000000001</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E203">
+        <v>79</v>
+      </c>
+      <c r="F203">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>687</v>
       </c>
@@ -4460,8 +4576,14 @@
       <c r="D204">
         <v>7.3869999999999996</v>
       </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E204">
+        <v>29</v>
+      </c>
+      <c r="F204">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>688</v>
       </c>
@@ -4474,8 +4596,14 @@
       <c r="D205">
         <v>8.7609999999999992</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E205">
+        <v>31</v>
+      </c>
+      <c r="F205">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>689</v>
       </c>
@@ -4488,8 +4616,14 @@
       <c r="D206">
         <v>8.2270000000000003</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E206">
+        <v>21</v>
+      </c>
+      <c r="F206">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>690</v>
       </c>
@@ -4502,8 +4636,14 @@
       <c r="D207">
         <v>13.039</v>
       </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E207">
+        <v>5</v>
+      </c>
+      <c r="F207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>691</v>
       </c>
@@ -4516,8 +4656,14 @@
       <c r="D208">
         <v>22.07</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E208">
+        <v>69</v>
+      </c>
+      <c r="F208">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>692</v>
       </c>
@@ -4530,8 +4676,14 @@
       <c r="D209">
         <v>21.780999999999999</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E209">
+        <v>34</v>
+      </c>
+      <c r="F209">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>693</v>
       </c>
@@ -4544,8 +4696,14 @@
       <c r="D210">
         <v>8.6850000000000005</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E210">
+        <v>42</v>
+      </c>
+      <c r="F210">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>694</v>
       </c>
@@ -4558,8 +4716,14 @@
       <c r="D211">
         <v>5.5620000000000003</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E211">
+        <v>73</v>
+      </c>
+      <c r="F211">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>695</v>
       </c>
@@ -4572,8 +4736,14 @@
       <c r="D212">
         <v>7.7770000000000001</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E212">
+        <v>2</v>
+      </c>
+      <c r="F212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>696</v>
       </c>
@@ -4586,8 +4756,14 @@
       <c r="D213">
         <v>9.4190000000000005</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E213">
+        <v>80</v>
+      </c>
+      <c r="F213">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>697</v>
       </c>
@@ -4600,8 +4776,14 @@
       <c r="D214">
         <v>17.087</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E214">
+        <v>78</v>
+      </c>
+      <c r="F214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>698</v>
       </c>
@@ -4614,8 +4796,14 @@
       <c r="D215">
         <v>28.683</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E215">
+        <v>27</v>
+      </c>
+      <c r="F215">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>699</v>
       </c>
@@ -4628,8 +4816,14 @@
       <c r="D216">
         <v>7.04</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E216">
+        <v>0</v>
+      </c>
+      <c r="F216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>700</v>
       </c>
@@ -4642,8 +4836,14 @@
       <c r="D217">
         <v>5.0659999999999998</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E217">
+        <v>34</v>
+      </c>
+      <c r="F217">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>701</v>
       </c>
@@ -4656,8 +4856,14 @@
       <c r="D218">
         <v>6.5949999999999998</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E218">
+        <v>2</v>
+      </c>
+      <c r="F218">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>702</v>
       </c>
@@ -4670,8 +4876,14 @@
       <c r="D219">
         <v>8.34</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E219">
+        <v>30</v>
+      </c>
+      <c r="F219">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>703</v>
       </c>
@@ -4684,8 +4896,14 @@
       <c r="D220">
         <v>7.86</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E220">
+        <v>51</v>
+      </c>
+      <c r="F220">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>704</v>
       </c>
@@ -4698,8 +4916,14 @@
       <c r="D221">
         <v>10.903</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E221">
+        <v>90</v>
+      </c>
+      <c r="F221">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>705</v>
       </c>
@@ -4712,8 +4936,14 @@
       <c r="D222">
         <v>8.859</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E222">
+        <v>74</v>
+      </c>
+      <c r="F222">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>706</v>
       </c>
@@ -4726,8 +4956,14 @@
       <c r="D223">
         <v>6.7080000000000002</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E223">
+        <v>63</v>
+      </c>
+      <c r="F223">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>707</v>
       </c>
@@ -4740,8 +4976,14 @@
       <c r="D224">
         <v>7.3159999999999998</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E224">
+        <v>1</v>
+      </c>
+      <c r="F224">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>708</v>
       </c>
@@ -4754,8 +4996,14 @@
       <c r="D225">
         <v>5.7809999999999997</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E225">
+        <v>86</v>
+      </c>
+      <c r="F225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>709</v>
       </c>
@@ -4768,8 +5016,14 @@
       <c r="D226">
         <v>4.5579999999999998</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E226">
+        <v>92</v>
+      </c>
+      <c r="F226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>710</v>
       </c>
@@ -4782,8 +5036,14 @@
       <c r="D227">
         <v>4.8209999999999997</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E227">
+        <v>157</v>
+      </c>
+      <c r="F227">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>711</v>
       </c>
@@ -4796,8 +5056,14 @@
       <c r="D228">
         <v>5.7220000000000004</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E228">
+        <v>35</v>
+      </c>
+      <c r="F228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>712</v>
       </c>
@@ -4810,8 +5076,14 @@
       <c r="D229">
         <v>9.3190000000000008</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E229">
+        <v>13</v>
+      </c>
+      <c r="F229">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>713</v>
       </c>
@@ -4824,8 +5096,14 @@
       <c r="D230">
         <v>8.8699999999999992</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E230">
+        <v>43</v>
+      </c>
+      <c r="F230">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>714</v>
       </c>
@@ -4838,8 +5116,14 @@
       <c r="D231">
         <v>9.3049999999999997</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E231">
+        <v>1</v>
+      </c>
+      <c r="F231">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>715</v>
       </c>
@@ -4852,8 +5136,14 @@
       <c r="D232">
         <v>9.5079999999999991</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E232">
+        <v>103</v>
+      </c>
+      <c r="F232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>716</v>
       </c>
@@ -4866,8 +5156,14 @@
       <c r="D233">
         <v>7.6550000000000002</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E233">
+        <v>63</v>
+      </c>
+      <c r="F233">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>717</v>
       </c>
@@ -4880,8 +5176,14 @@
       <c r="D234">
         <v>10.593999999999999</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E234">
+        <v>47</v>
+      </c>
+      <c r="F234">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>718</v>
       </c>
@@ -4894,8 +5196,14 @@
       <c r="D235">
         <v>6.234</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E235">
+        <v>62</v>
+      </c>
+      <c r="F235">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>719</v>
       </c>
@@ -4908,8 +5216,14 @@
       <c r="D236">
         <v>9.6590000000000007</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E236">
+        <v>2</v>
+      </c>
+      <c r="F236">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>720</v>
       </c>
@@ -4922,8 +5236,14 @@
       <c r="D237">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E237">
+        <v>127</v>
+      </c>
+      <c r="F237">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>721</v>
       </c>
@@ -4936,8 +5256,14 @@
       <c r="D238">
         <v>9.6180000000000003</v>
       </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E238">
+        <v>70</v>
+      </c>
+      <c r="F238">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>722</v>
       </c>
@@ -4950,8 +5276,14 @@
       <c r="D239">
         <v>6.306</v>
       </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E239">
+        <v>126</v>
+      </c>
+      <c r="F239">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>723</v>
       </c>
@@ -4964,8 +5296,14 @@
       <c r="D240">
         <v>6.835</v>
       </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E240">
+        <v>1</v>
+      </c>
+      <c r="F240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>724</v>
       </c>
@@ -4978,8 +5316,14 @@
       <c r="D241">
         <v>7.9249999999999998</v>
       </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E241">
+        <v>30</v>
+      </c>
+      <c r="F241">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>725</v>
       </c>
@@ -4992,8 +5336,14 @@
       <c r="D242">
         <v>9.1820000000000004</v>
       </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E242">
+        <v>0</v>
+      </c>
+      <c r="F242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>726</v>
       </c>
@@ -5006,8 +5356,14 @@
       <c r="D243">
         <v>7.8730000000000002</v>
       </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E243">
+        <v>40</v>
+      </c>
+      <c r="F243">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>727</v>
       </c>
@@ -5020,8 +5376,14 @@
       <c r="D244">
         <v>6.7830000000000004</v>
       </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E244">
+        <v>59</v>
+      </c>
+      <c r="F244">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>728</v>
       </c>
@@ -5034,8 +5396,14 @@
       <c r="D245">
         <v>5.5430000000000001</v>
       </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E245">
+        <v>15</v>
+      </c>
+      <c r="F245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>729</v>
       </c>
@@ -5048,8 +5416,14 @@
       <c r="D246">
         <v>8.3170000000000002</v>
       </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E246">
+        <v>62</v>
+      </c>
+      <c r="F246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>730</v>
       </c>
@@ -5062,8 +5436,14 @@
       <c r="D247">
         <v>8.02</v>
       </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E247">
+        <v>47</v>
+      </c>
+      <c r="F247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>731</v>
       </c>
@@ -5076,8 +5456,14 @@
       <c r="D248">
         <v>5.3209999999999997</v>
       </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E248">
+        <v>0</v>
+      </c>
+      <c r="F248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>732</v>
       </c>
@@ -5090,8 +5476,14 @@
       <c r="D249">
         <v>6.992</v>
       </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E249">
+        <v>57</v>
+      </c>
+      <c r="F249">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>733</v>
       </c>
@@ -5104,8 +5496,14 @@
       <c r="D250">
         <v>5.383</v>
       </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E250">
+        <v>96</v>
+      </c>
+      <c r="F250">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>734</v>
       </c>
@@ -5118,8 +5516,14 @@
       <c r="D251">
         <v>7.327</v>
       </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E251">
+        <v>40</v>
+      </c>
+      <c r="F251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>735</v>
       </c>
@@ -5132,8 +5536,14 @@
       <c r="D252">
         <v>4.6959999999999997</v>
       </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E252">
+        <v>28</v>
+      </c>
+      <c r="F252">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>736</v>
       </c>
@@ -5146,8 +5556,14 @@
       <c r="D253">
         <v>5.9409999999999998</v>
       </c>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E253">
+        <v>7</v>
+      </c>
+      <c r="F253">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>737</v>
       </c>
@@ -5160,8 +5576,14 @@
       <c r="D254">
         <v>6.8029999999999999</v>
       </c>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E254">
+        <v>19</v>
+      </c>
+      <c r="F254">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>738</v>
       </c>
@@ -5174,8 +5596,14 @@
       <c r="D255">
         <v>6.843</v>
       </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E255">
+        <v>58</v>
+      </c>
+      <c r="F255">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>739</v>
       </c>
@@ -5188,8 +5616,14 @@
       <c r="D256">
         <v>7.4279999999999999</v>
       </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E256">
+        <v>22</v>
+      </c>
+      <c r="F256">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>740</v>
       </c>
@@ -5202,8 +5636,14 @@
       <c r="D257">
         <v>6.5149999999999997</v>
       </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E257">
+        <v>86</v>
+      </c>
+      <c r="F257">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>741</v>
       </c>
@@ -5216,8 +5656,14 @@
       <c r="D258">
         <v>6.7130000000000001</v>
       </c>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E258">
+        <v>33</v>
+      </c>
+      <c r="F258">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>742</v>
       </c>
@@ -5230,8 +5676,14 @@
       <c r="D259">
         <v>7.1139999999999999</v>
       </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E259">
+        <v>43</v>
+      </c>
+      <c r="F259">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>743</v>
       </c>
@@ -5244,8 +5696,14 @@
       <c r="D260">
         <v>8.3559999999999999</v>
       </c>
-    </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E260">
+        <v>5</v>
+      </c>
+      <c r="F260">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>744</v>
       </c>
@@ -5258,8 +5716,14 @@
       <c r="D261">
         <v>6.3849999999999998</v>
       </c>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E261">
+        <v>93</v>
+      </c>
+      <c r="F261">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>745</v>
       </c>
@@ -5272,8 +5736,14 @@
       <c r="D262">
         <v>3.7909999999999999</v>
       </c>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E262">
+        <v>91</v>
+      </c>
+      <c r="F262">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>746</v>
       </c>
@@ -5286,8 +5756,14 @@
       <c r="D263">
         <v>8.2129999999999992</v>
       </c>
-    </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E263">
+        <v>41</v>
+      </c>
+      <c r="F263">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>747</v>
       </c>
@@ -5300,8 +5776,14 @@
       <c r="D264">
         <v>6.1680000000000001</v>
       </c>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E264">
+        <v>0</v>
+      </c>
+      <c r="F264">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>748</v>
       </c>
@@ -5314,8 +5796,14 @@
       <c r="D265">
         <v>4.5609999999999999</v>
       </c>
-    </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E265">
+        <v>17</v>
+      </c>
+      <c r="F265">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>749</v>
       </c>
@@ -5329,7 +5817,7 @@
         <v>4.5730000000000004</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>750</v>
       </c>
@@ -5343,7 +5831,7 @@
         <v>8.3209999999999997</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>751</v>
       </c>
@@ -5357,7 +5845,7 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>752</v>
       </c>
@@ -5371,7 +5859,7 @@
         <v>7.3360000000000003</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>753</v>
       </c>
@@ -5385,7 +5873,7 @@
         <v>8.4480000000000004</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>754</v>
       </c>
@@ -5399,7 +5887,7 @@
         <v>4.2549999999999999</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>755</v>
       </c>
@@ -5413,7 +5901,7 @@
         <v>8.9269999999999996</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>756</v>
       </c>
@@ -5427,7 +5915,7 @@
         <v>6.8959999999999999</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>757</v>
       </c>
@@ -5441,7 +5929,7 @@
         <v>8.9149999999999991</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>758</v>
       </c>
@@ -5455,7 +5943,7 @@
         <v>7.827</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>759</v>
       </c>
@@ -5469,7 +5957,7 @@
         <v>6.4660000000000002</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>760</v>
       </c>
@@ -5483,7 +5971,7 @@
         <v>7.3179999999999996</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>761</v>
       </c>
@@ -5497,7 +5985,7 @@
         <v>5.5389999999999997</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>762</v>
       </c>
@@ -5511,7 +5999,7 @@
         <v>7.0019999999999998</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>763</v>
       </c>
@@ -5525,7 +6013,7 @@
         <v>1.534</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>764</v>
       </c>
@@ -5539,7 +6027,7 @@
         <v>3.7429999999999999</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>765</v>
       </c>
@@ -5553,7 +6041,7 @@
         <v>4.2709999999999999</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>766</v>
       </c>
@@ -5567,7 +6055,7 @@
         <v>3.508</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>767</v>
       </c>
@@ -5581,7 +6069,7 @@
         <v>5.1040000000000001</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>768</v>
       </c>
@@ -5595,7 +6083,7 @@
         <v>2.1819999999999999</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>769</v>
       </c>
@@ -5609,7 +6097,7 @@
         <v>2.8969999999999998</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>770</v>
       </c>
@@ -5623,7 +6111,7 @@
         <v>2.3980000000000001</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>771</v>
       </c>
@@ -5637,7 +6125,7 @@
         <v>2.5499999999999998</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>772</v>
       </c>
@@ -5651,13 +6139,13 @@
         <v>3.0190000000000001</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C290" s="1"/>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C291" s="1"/>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C292" s="1"/>
     </row>
   </sheetData>

</xml_diff>